<commit_message>
Added references and comments
</commit_message>
<xml_diff>
--- a/Prototypes/Oats/Observed/Oats_rainshelter_9899.xlsx
+++ b/Prototypes/Oats/Observed/Oats_rainshelter_9899.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385" activeTab="1"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="11385"/>
   </bookViews>
   <sheets>
     <sheet name="Observations" sheetId="1" r:id="rId1"/>
@@ -60,15 +60,6 @@
     <t>Clock.Today</t>
   </si>
   <si>
-    <t>Oats.Stem.Live.Wt</t>
-  </si>
-  <si>
-    <t>Oats.Leaf.Live.Wt</t>
-  </si>
-  <si>
-    <t>Oats.Grain.Live.Wt</t>
-  </si>
-  <si>
     <t>Oats.Height</t>
   </si>
   <si>
@@ -88,9 +79,6 @@
   </si>
   <si>
     <t>Oats.Leaf.Dead.Wt</t>
-  </si>
-  <si>
-    <t>Oats.AbovegroundLive.Wt</t>
   </si>
   <si>
     <t>Oats.Leaf.LAI</t>
@@ -145,6 +133,18 @@
   </si>
   <si>
     <t>Oats.Structure.LeafTipsAppeared</t>
+  </si>
+  <si>
+    <t>Oats.Aboveground.Wt</t>
+  </si>
+  <si>
+    <t>Oats.Grain.Wt</t>
+  </si>
+  <si>
+    <t>Oats.Leaf.Wt</t>
+  </si>
+  <si>
+    <t>Oats.Stem.Wt</t>
   </si>
 </sst>
 </file>
@@ -473,8 +473,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:P181"/>
   <sheetViews>
-    <sheetView topLeftCell="A149" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="D1" sqref="D1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="21.140625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -491,57 +491,57 @@
   <sheetData>
     <row r="1" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>38</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>16</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="L1" s="1" t="s">
         <v>11</v>
       </c>
-      <c r="E1" s="1" t="s">
+      <c r="M1" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="N1" s="1" t="s">
         <v>12</v>
       </c>
-      <c r="F1" s="1" t="s">
+      <c r="O1" s="1" t="s">
         <v>13</v>
       </c>
-      <c r="G1" s="1" t="s">
-        <v>18</v>
-      </c>
-      <c r="H1" s="1" t="s">
-        <v>19</v>
-      </c>
-      <c r="I1" s="1" t="s">
-        <v>20</v>
-      </c>
-      <c r="J1" s="1" t="s">
-        <v>21</v>
-      </c>
-      <c r="K1" s="1" t="s">
-        <v>22</v>
-      </c>
-      <c r="L1" s="1" t="s">
+      <c r="P1" s="1" t="s">
         <v>14</v>
-      </c>
-      <c r="M1" s="1" t="s">
-        <v>23</v>
-      </c>
-      <c r="N1" s="1" t="s">
-        <v>15</v>
-      </c>
-      <c r="O1" s="1" t="s">
-        <v>16</v>
-      </c>
-      <c r="P1" s="1" t="s">
-        <v>17</v>
       </c>
     </row>
     <row r="2" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -582,7 +582,7 @@
     </row>
     <row r="3" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -623,7 +623,7 @@
     </row>
     <row r="4" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -664,7 +664,7 @@
     </row>
     <row r="5" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -705,7 +705,7 @@
     </row>
     <row r="6" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -746,7 +746,7 @@
     </row>
     <row r="7" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -787,7 +787,7 @@
     </row>
     <row r="8" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -828,7 +828,7 @@
     </row>
     <row r="9" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -869,7 +869,7 @@
     </row>
     <row r="10" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -910,7 +910,7 @@
     </row>
     <row r="11" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -951,7 +951,7 @@
     </row>
     <row r="12" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -992,7 +992,7 @@
     </row>
     <row r="13" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -1033,7 +1033,7 @@
     </row>
     <row r="14" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -1074,7 +1074,7 @@
     </row>
     <row r="15" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -1115,7 +1115,7 @@
     </row>
     <row r="16" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -1156,7 +1156,7 @@
     </row>
     <row r="17" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -1197,7 +1197,7 @@
     </row>
     <row r="18" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -1238,7 +1238,7 @@
     </row>
     <row r="19" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -1279,7 +1279,7 @@
     </row>
     <row r="20" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -1320,7 +1320,7 @@
     </row>
     <row r="21" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -1361,7 +1361,7 @@
     </row>
     <row r="22" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -1402,7 +1402,7 @@
     </row>
     <row r="23" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -1443,7 +1443,7 @@
     </row>
     <row r="24" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
@@ -1484,7 +1484,7 @@
     </row>
     <row r="25" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -1525,7 +1525,7 @@
     </row>
     <row r="26" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -1566,7 +1566,7 @@
     </row>
     <row r="27" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -1607,7 +1607,7 @@
     </row>
     <row r="28" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
@@ -1648,7 +1648,7 @@
     </row>
     <row r="29" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -1689,7 +1689,7 @@
     </row>
     <row r="30" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -1730,7 +1730,7 @@
     </row>
     <row r="31" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
@@ -1771,7 +1771,7 @@
     </row>
     <row r="32" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
@@ -1812,7 +1812,7 @@
     </row>
     <row r="33" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -1853,7 +1853,7 @@
     </row>
     <row r="34" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -1894,7 +1894,7 @@
     </row>
     <row r="35" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
@@ -1935,7 +1935,7 @@
     </row>
     <row r="36" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>2</v>
@@ -1976,7 +1976,7 @@
     </row>
     <row r="37" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
@@ -2017,7 +2017,7 @@
     </row>
     <row r="38" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
@@ -2058,7 +2058,7 @@
     </row>
     <row r="39" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -2099,7 +2099,7 @@
     </row>
     <row r="40" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
@@ -2140,7 +2140,7 @@
     </row>
     <row r="41" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -2181,7 +2181,7 @@
     </row>
     <row r="42" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>8</v>
@@ -2222,7 +2222,7 @@
     </row>
     <row r="43" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>9</v>
@@ -2263,7 +2263,7 @@
     </row>
     <row r="44" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>0</v>
@@ -2304,7 +2304,7 @@
     </row>
     <row r="45" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>1</v>
@@ -2345,7 +2345,7 @@
     </row>
     <row r="46" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>2</v>
@@ -2386,7 +2386,7 @@
     </row>
     <row r="47" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>3</v>
@@ -2427,7 +2427,7 @@
     </row>
     <row r="48" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
@@ -2468,7 +2468,7 @@
     </row>
     <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -2509,7 +2509,7 @@
     </row>
     <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
@@ -2550,7 +2550,7 @@
     </row>
     <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -2591,7 +2591,7 @@
     </row>
     <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
@@ -2632,7 +2632,7 @@
     </row>
     <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>9</v>
@@ -2676,7 +2676,7 @@
     </row>
     <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>0</v>
@@ -2714,7 +2714,7 @@
     </row>
     <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>1</v>
@@ -2758,7 +2758,7 @@
     </row>
     <row r="56" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>2</v>
@@ -2802,7 +2802,7 @@
     </row>
     <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>3</v>
@@ -2846,7 +2846,7 @@
     </row>
     <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>4</v>
@@ -2890,7 +2890,7 @@
     </row>
     <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
@@ -2928,7 +2928,7 @@
     </row>
     <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
@@ -2966,7 +2966,7 @@
     </row>
     <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
@@ -3004,7 +3004,7 @@
     </row>
     <row r="62" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>8</v>
@@ -3054,7 +3054,7 @@
     </row>
     <row r="63" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>9</v>
@@ -3104,7 +3104,7 @@
     </row>
     <row r="64" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>0</v>
@@ -3154,7 +3154,7 @@
     </row>
     <row r="65" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>1</v>
@@ -3204,7 +3204,7 @@
     </row>
     <row r="66" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>2</v>
@@ -3254,7 +3254,7 @@
     </row>
     <row r="67" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
@@ -3304,7 +3304,7 @@
     </row>
     <row r="68" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -3354,7 +3354,7 @@
     </row>
     <row r="69" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -3404,7 +3404,7 @@
     </row>
     <row r="70" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
@@ -3442,7 +3442,7 @@
     </row>
     <row r="71" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
@@ -3492,7 +3492,7 @@
     </row>
     <row r="72" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
@@ -3542,7 +3542,7 @@
     </row>
     <row r="73" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>9</v>
@@ -3592,7 +3592,7 @@
     </row>
     <row r="74" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>0</v>
@@ -3642,7 +3642,7 @@
     </row>
     <row r="75" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1</v>
@@ -3692,7 +3692,7 @@
     </row>
     <row r="76" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>2</v>
@@ -3742,7 +3742,7 @@
     </row>
     <row r="77" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>3</v>
@@ -3792,7 +3792,7 @@
     </row>
     <row r="78" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
@@ -3842,7 +3842,7 @@
     </row>
     <row r="79" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
@@ -3892,7 +3892,7 @@
     </row>
     <row r="80" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -3942,7 +3942,7 @@
     </row>
     <row r="81" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
@@ -3992,7 +3992,7 @@
     </row>
     <row r="82" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>8</v>
@@ -4042,7 +4042,7 @@
     </row>
     <row r="83" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>9</v>
@@ -4092,7 +4092,7 @@
     </row>
     <row r="84" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>0</v>
@@ -4142,7 +4142,7 @@
     </row>
     <row r="85" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>1</v>
@@ -4192,7 +4192,7 @@
     </row>
     <row r="86" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>2</v>
@@ -4242,7 +4242,7 @@
     </row>
     <row r="87" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>3</v>
@@ -4292,7 +4292,7 @@
     </row>
     <row r="88" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -4342,7 +4342,7 @@
     </row>
     <row r="89" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
@@ -4392,7 +4392,7 @@
     </row>
     <row r="90" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -4442,7 +4442,7 @@
     </row>
     <row r="91" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>7</v>
@@ -4492,7 +4492,7 @@
     </row>
     <row r="92" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>8</v>
@@ -4542,7 +4542,7 @@
     </row>
     <row r="93" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>9</v>
@@ -4592,7 +4592,7 @@
     </row>
     <row r="94" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>0</v>
@@ -4642,7 +4642,7 @@
     </row>
     <row r="95" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>1</v>
@@ -4692,7 +4692,7 @@
     </row>
     <row r="96" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>2</v>
@@ -4742,7 +4742,7 @@
     </row>
     <row r="97" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>3</v>
@@ -4792,7 +4792,7 @@
     </row>
     <row r="98" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
@@ -4842,7 +4842,7 @@
     </row>
     <row r="99" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
@@ -4892,7 +4892,7 @@
     </row>
     <row r="100" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>6</v>
@@ -4942,7 +4942,7 @@
     </row>
     <row r="101" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>7</v>
@@ -4992,7 +4992,7 @@
     </row>
     <row r="102" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>8</v>
@@ -5042,7 +5042,7 @@
     </row>
     <row r="103" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>9</v>
@@ -5089,7 +5089,7 @@
     </row>
     <row r="104" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>0</v>
@@ -5139,7 +5139,7 @@
     </row>
     <row r="105" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>1</v>
@@ -5189,7 +5189,7 @@
     </row>
     <row r="106" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>2</v>
@@ -5239,7 +5239,7 @@
     </row>
     <row r="107" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>3</v>
@@ -5289,7 +5289,7 @@
     </row>
     <row r="108" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>4</v>
@@ -5336,7 +5336,7 @@
     </row>
     <row r="109" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
@@ -5386,7 +5386,7 @@
     </row>
     <row r="110" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>6</v>
@@ -5436,7 +5436,7 @@
     </row>
     <row r="111" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
@@ -5486,7 +5486,7 @@
     </row>
     <row r="112" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>8</v>
@@ -5533,7 +5533,7 @@
     </row>
     <row r="113" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>9</v>
@@ -5577,7 +5577,7 @@
     </row>
     <row r="114" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>0</v>
@@ -5624,7 +5624,7 @@
     </row>
     <row r="115" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>1</v>
@@ -5671,7 +5671,7 @@
     </row>
     <row r="116" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>2</v>
@@ -5718,7 +5718,7 @@
     </row>
     <row r="117" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>3</v>
@@ -5765,7 +5765,7 @@
     </row>
     <row r="118" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>4</v>
@@ -5809,7 +5809,7 @@
     </row>
     <row r="119" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>5</v>
@@ -5853,7 +5853,7 @@
     </row>
     <row r="120" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>6</v>
@@ -5897,7 +5897,7 @@
     </row>
     <row r="121" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
@@ -5944,7 +5944,7 @@
     </row>
     <row r="122" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>8</v>
@@ -5991,7 +5991,7 @@
     </row>
     <row r="123" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>9</v>
@@ -6035,7 +6035,7 @@
     </row>
     <row r="124" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>0</v>
@@ -6082,7 +6082,7 @@
     </row>
     <row r="125" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>1</v>
@@ -6129,7 +6129,7 @@
     </row>
     <row r="126" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>2</v>
@@ -6176,7 +6176,7 @@
     </row>
     <row r="127" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>3</v>
@@ -6223,7 +6223,7 @@
     </row>
     <row r="128" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>4</v>
@@ -6267,7 +6267,7 @@
     </row>
     <row r="129" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
@@ -6311,7 +6311,7 @@
     </row>
     <row r="130" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>6</v>
@@ -6355,7 +6355,7 @@
     </row>
     <row r="131" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>7</v>
@@ -6399,7 +6399,7 @@
     </row>
     <row r="132" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>8</v>
@@ -6446,7 +6446,7 @@
     </row>
     <row r="133" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>9</v>
@@ -6490,7 +6490,7 @@
     </row>
     <row r="134" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>0</v>
@@ -6537,7 +6537,7 @@
     </row>
     <row r="135" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>1</v>
@@ -6584,7 +6584,7 @@
     </row>
     <row r="136" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>2</v>
@@ -6631,7 +6631,7 @@
     </row>
     <row r="137" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>3</v>
@@ -6678,7 +6678,7 @@
     </row>
     <row r="138" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>4</v>
@@ -6722,7 +6722,7 @@
     </row>
     <row r="139" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
@@ -6766,7 +6766,7 @@
     </row>
     <row r="140" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>6</v>
@@ -6810,7 +6810,7 @@
     </row>
     <row r="141" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
@@ -6854,7 +6854,7 @@
     </row>
     <row r="142" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>8</v>
@@ -6901,7 +6901,7 @@
     </row>
     <row r="143" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>9</v>
@@ -6924,7 +6924,7 @@
     </row>
     <row r="144" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>0</v>
@@ -6971,7 +6971,7 @@
     </row>
     <row r="145" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>1</v>
@@ -7018,7 +7018,7 @@
     </row>
     <row r="146" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>2</v>
@@ -7065,7 +7065,7 @@
     </row>
     <row r="147" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>3</v>
@@ -7112,7 +7112,7 @@
     </row>
     <row r="148" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>4</v>
@@ -7135,7 +7135,7 @@
     </row>
     <row r="149" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>5</v>
@@ -7158,7 +7158,7 @@
     </row>
     <row r="150" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>6</v>
@@ -7181,7 +7181,7 @@
     </row>
     <row r="151" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>7</v>
@@ -7204,7 +7204,7 @@
     </row>
     <row r="152" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>8</v>
@@ -7251,7 +7251,7 @@
     </row>
     <row r="153" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>9</v>
@@ -7271,7 +7271,7 @@
     </row>
     <row r="154" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>0</v>
@@ -7318,7 +7318,7 @@
     </row>
     <row r="155" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>1</v>
@@ -7365,7 +7365,7 @@
     </row>
     <row r="156" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>2</v>
@@ -7412,7 +7412,7 @@
     </row>
     <row r="157" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>3</v>
@@ -7459,7 +7459,7 @@
     </row>
     <row r="158" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>4</v>
@@ -7479,7 +7479,7 @@
     </row>
     <row r="159" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>5</v>
@@ -7499,7 +7499,7 @@
     </row>
     <row r="160" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>6</v>
@@ -7519,7 +7519,7 @@
     </row>
     <row r="161" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>7</v>
@@ -7539,7 +7539,7 @@
     </row>
     <row r="162" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>8</v>
@@ -7586,7 +7586,7 @@
     </row>
     <row r="163" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>9</v>
@@ -7606,7 +7606,7 @@
     </row>
     <row r="164" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>0</v>
@@ -7653,7 +7653,7 @@
     </row>
     <row r="165" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>1</v>
@@ -7700,7 +7700,7 @@
     </row>
     <row r="166" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>2</v>
@@ -7747,7 +7747,7 @@
     </row>
     <row r="167" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>3</v>
@@ -7794,7 +7794,7 @@
     </row>
     <row r="168" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>4</v>
@@ -7814,7 +7814,7 @@
     </row>
     <row r="169" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>5</v>
@@ -7834,7 +7834,7 @@
     </row>
     <row r="170" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>6</v>
@@ -7854,7 +7854,7 @@
     </row>
     <row r="171" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>7</v>
@@ -7874,7 +7874,7 @@
     </row>
     <row r="172" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>8</v>
@@ -7918,7 +7918,7 @@
     </row>
     <row r="173" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>9</v>
@@ -7938,7 +7938,7 @@
     </row>
     <row r="174" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>0</v>
@@ -7985,7 +7985,7 @@
     </row>
     <row r="175" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>1</v>
@@ -8032,7 +8032,7 @@
     </row>
     <row r="176" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>2</v>
@@ -8079,7 +8079,7 @@
     </row>
     <row r="177" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>3</v>
@@ -8126,7 +8126,7 @@
     </row>
     <row r="178" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>4</v>
@@ -8146,7 +8146,7 @@
     </row>
     <row r="179" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
@@ -8166,7 +8166,7 @@
     </row>
     <row r="180" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
@@ -8186,7 +8186,7 @@
     </row>
     <row r="181" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>7</v>
@@ -8214,7 +8214,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:G191"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr defaultColWidth="19.28515625" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -8230,30 +8230,30 @@
   <sheetData>
     <row r="1" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="C1" s="2" t="s">
         <v>10</v>
       </c>
       <c r="D1" s="1" t="s">
-        <v>39</v>
+        <v>35</v>
       </c>
       <c r="E1" s="1" t="s">
-        <v>36</v>
+        <v>32</v>
       </c>
       <c r="F1" s="1" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="G1" s="1" t="s">
-        <v>38</v>
+        <v>34</v>
       </c>
     </row>
     <row r="2" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>8</v>
@@ -8276,7 +8276,7 @@
     </row>
     <row r="3" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B3" s="1" t="s">
         <v>9</v>
@@ -8299,7 +8299,7 @@
     </row>
     <row r="4" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A4" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B4" s="1" t="s">
         <v>0</v>
@@ -8322,7 +8322,7 @@
     </row>
     <row r="5" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A5" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B5" s="1" t="s">
         <v>1</v>
@@ -8345,7 +8345,7 @@
     </row>
     <row r="6" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A6" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B6" s="1" t="s">
         <v>2</v>
@@ -8368,7 +8368,7 @@
     </row>
     <row r="7" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A7" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B7" s="1" t="s">
         <v>3</v>
@@ -8391,7 +8391,7 @@
     </row>
     <row r="8" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A8" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B8" s="1" t="s">
         <v>4</v>
@@ -8414,7 +8414,7 @@
     </row>
     <row r="9" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A9" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B9" s="1" t="s">
         <v>5</v>
@@ -8437,7 +8437,7 @@
     </row>
     <row r="10" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A10" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B10" s="1" t="s">
         <v>6</v>
@@ -8460,7 +8460,7 @@
     </row>
     <row r="11" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A11" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B11" s="1" t="s">
         <v>7</v>
@@ -8483,7 +8483,7 @@
     </row>
     <row r="12" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A12" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B12" s="1" t="s">
         <v>8</v>
@@ -8506,7 +8506,7 @@
     </row>
     <row r="13" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A13" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B13" s="1" t="s">
         <v>9</v>
@@ -8529,7 +8529,7 @@
     </row>
     <row r="14" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A14" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B14" s="1" t="s">
         <v>0</v>
@@ -8552,7 +8552,7 @@
     </row>
     <row r="15" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A15" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B15" s="1" t="s">
         <v>1</v>
@@ -8575,7 +8575,7 @@
     </row>
     <row r="16" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A16" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B16" s="1" t="s">
         <v>2</v>
@@ -8598,7 +8598,7 @@
     </row>
     <row r="17" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A17" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B17" s="1" t="s">
         <v>3</v>
@@ -8621,7 +8621,7 @@
     </row>
     <row r="18" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A18" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B18" s="1" t="s">
         <v>4</v>
@@ -8644,7 +8644,7 @@
     </row>
     <row r="19" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A19" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B19" s="1" t="s">
         <v>5</v>
@@ -8667,7 +8667,7 @@
     </row>
     <row r="20" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A20" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B20" s="1" t="s">
         <v>6</v>
@@ -8690,7 +8690,7 @@
     </row>
     <row r="21" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A21" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B21" s="1" t="s">
         <v>7</v>
@@ -8713,7 +8713,7 @@
     </row>
     <row r="22" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A22" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B22" s="1" t="s">
         <v>8</v>
@@ -8736,7 +8736,7 @@
     </row>
     <row r="23" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A23" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B23" s="1" t="s">
         <v>9</v>
@@ -8759,7 +8759,7 @@
     </row>
     <row r="24" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A24" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B24" s="1" t="s">
         <v>0</v>
@@ -8782,7 +8782,7 @@
     </row>
     <row r="25" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A25" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B25" s="1" t="s">
         <v>1</v>
@@ -8805,7 +8805,7 @@
     </row>
     <row r="26" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A26" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B26" s="1" t="s">
         <v>2</v>
@@ -8828,7 +8828,7 @@
     </row>
     <row r="27" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A27" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B27" s="1" t="s">
         <v>3</v>
@@ -8851,7 +8851,7 @@
     </row>
     <row r="28" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A28" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B28" s="1" t="s">
         <v>4</v>
@@ -8874,7 +8874,7 @@
     </row>
     <row r="29" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A29" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B29" s="1" t="s">
         <v>5</v>
@@ -8897,7 +8897,7 @@
     </row>
     <row r="30" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A30" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B30" s="1" t="s">
         <v>6</v>
@@ -8920,7 +8920,7 @@
     </row>
     <row r="31" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A31" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B31" s="1" t="s">
         <v>7</v>
@@ -8943,7 +8943,7 @@
     </row>
     <row r="32" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A32" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B32" s="1" t="s">
         <v>8</v>
@@ -8966,7 +8966,7 @@
     </row>
     <row r="33" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A33" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B33" s="1" t="s">
         <v>9</v>
@@ -8989,7 +8989,7 @@
     </row>
     <row r="34" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A34" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B34" s="1" t="s">
         <v>0</v>
@@ -9012,7 +9012,7 @@
     </row>
     <row r="35" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A35" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B35" s="1" t="s">
         <v>1</v>
@@ -9035,7 +9035,7 @@
     </row>
     <row r="36" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A36" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B36" s="1" t="s">
         <v>2</v>
@@ -9058,7 +9058,7 @@
     </row>
     <row r="37" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A37" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B37" s="1" t="s">
         <v>3</v>
@@ -9081,7 +9081,7 @@
     </row>
     <row r="38" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A38" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B38" s="1" t="s">
         <v>4</v>
@@ -9104,7 +9104,7 @@
     </row>
     <row r="39" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A39" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B39" s="1" t="s">
         <v>5</v>
@@ -9127,7 +9127,7 @@
     </row>
     <row r="40" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A40" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B40" s="1" t="s">
         <v>6</v>
@@ -9150,7 +9150,7 @@
     </row>
     <row r="41" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A41" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B41" s="1" t="s">
         <v>7</v>
@@ -9173,7 +9173,7 @@
     </row>
     <row r="42" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A42" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B42" s="1" t="s">
         <v>8</v>
@@ -9196,7 +9196,7 @@
     </row>
     <row r="43" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A43" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B43" s="1" t="s">
         <v>9</v>
@@ -9219,7 +9219,7 @@
     </row>
     <row r="44" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A44" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B44" s="1" t="s">
         <v>0</v>
@@ -9242,7 +9242,7 @@
     </row>
     <row r="45" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A45" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B45" s="1" t="s">
         <v>1</v>
@@ -9265,7 +9265,7 @@
     </row>
     <row r="46" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A46" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B46" s="1" t="s">
         <v>2</v>
@@ -9288,7 +9288,7 @@
     </row>
     <row r="47" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A47" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B47" s="1" t="s">
         <v>3</v>
@@ -9311,7 +9311,7 @@
     </row>
     <row r="48" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A48" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B48" s="1" t="s">
         <v>4</v>
@@ -9334,7 +9334,7 @@
     </row>
     <row r="49" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A49" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B49" s="1" t="s">
         <v>5</v>
@@ -9357,7 +9357,7 @@
     </row>
     <row r="50" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A50" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B50" s="1" t="s">
         <v>6</v>
@@ -9380,7 +9380,7 @@
     </row>
     <row r="51" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A51" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B51" s="1" t="s">
         <v>7</v>
@@ -9403,7 +9403,7 @@
     </row>
     <row r="52" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A52" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B52" s="1" t="s">
         <v>8</v>
@@ -9426,7 +9426,7 @@
     </row>
     <row r="53" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A53" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B53" s="1" t="s">
         <v>9</v>
@@ -9449,7 +9449,7 @@
     </row>
     <row r="54" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A54" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B54" s="1" t="s">
         <v>0</v>
@@ -9472,7 +9472,7 @@
     </row>
     <row r="55" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A55" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B55" s="1" t="s">
         <v>1</v>
@@ -9495,7 +9495,7 @@
     </row>
     <row r="56" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A56" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B56" s="1" t="s">
         <v>2</v>
@@ -9518,7 +9518,7 @@
     </row>
     <row r="57" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A57" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B57" s="1" t="s">
         <v>3</v>
@@ -9541,7 +9541,7 @@
     </row>
     <row r="58" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A58" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B58" s="1" t="s">
         <v>4</v>
@@ -9564,7 +9564,7 @@
     </row>
     <row r="59" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A59" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B59" s="1" t="s">
         <v>5</v>
@@ -9587,7 +9587,7 @@
     </row>
     <row r="60" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A60" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B60" s="1" t="s">
         <v>6</v>
@@ -9610,7 +9610,7 @@
     </row>
     <row r="61" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A61" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B61" s="1" t="s">
         <v>7</v>
@@ -9633,7 +9633,7 @@
     </row>
     <row r="62" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A62" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B62" s="1" t="s">
         <v>8</v>
@@ -9656,7 +9656,7 @@
     </row>
     <row r="63" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A63" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B63" s="1" t="s">
         <v>9</v>
@@ -9679,7 +9679,7 @@
     </row>
     <row r="64" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A64" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B64" s="1" t="s">
         <v>0</v>
@@ -9702,7 +9702,7 @@
     </row>
     <row r="65" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A65" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B65" s="1" t="s">
         <v>1</v>
@@ -9725,7 +9725,7 @@
     </row>
     <row r="66" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A66" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B66" s="1" t="s">
         <v>2</v>
@@ -9748,7 +9748,7 @@
     </row>
     <row r="67" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A67" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B67" s="1" t="s">
         <v>3</v>
@@ -9771,7 +9771,7 @@
     </row>
     <row r="68" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A68" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B68" s="1" t="s">
         <v>4</v>
@@ -9794,7 +9794,7 @@
     </row>
     <row r="69" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A69" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B69" s="1" t="s">
         <v>5</v>
@@ -9817,7 +9817,7 @@
     </row>
     <row r="70" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A70" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B70" s="1" t="s">
         <v>6</v>
@@ -9840,7 +9840,7 @@
     </row>
     <row r="71" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A71" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B71" s="1" t="s">
         <v>7</v>
@@ -9863,7 +9863,7 @@
     </row>
     <row r="72" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A72" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B72" s="1" t="s">
         <v>8</v>
@@ -9886,7 +9886,7 @@
     </row>
     <row r="73" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A73" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B73" s="1" t="s">
         <v>9</v>
@@ -9909,7 +9909,7 @@
     </row>
     <row r="74" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A74" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B74" s="1" t="s">
         <v>0</v>
@@ -9932,7 +9932,7 @@
     </row>
     <row r="75" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A75" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B75" s="1" t="s">
         <v>1</v>
@@ -9955,7 +9955,7 @@
     </row>
     <row r="76" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A76" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B76" s="1" t="s">
         <v>2</v>
@@ -9978,7 +9978,7 @@
     </row>
     <row r="77" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A77" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B77" s="1" t="s">
         <v>3</v>
@@ -10001,7 +10001,7 @@
     </row>
     <row r="78" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A78" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B78" s="1" t="s">
         <v>4</v>
@@ -10024,7 +10024,7 @@
     </row>
     <row r="79" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A79" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B79" s="1" t="s">
         <v>5</v>
@@ -10047,7 +10047,7 @@
     </row>
     <row r="80" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A80" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B80" s="1" t="s">
         <v>6</v>
@@ -10070,7 +10070,7 @@
     </row>
     <row r="81" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A81" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B81" s="1" t="s">
         <v>7</v>
@@ -10093,7 +10093,7 @@
     </row>
     <row r="82" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A82" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B82" s="1" t="s">
         <v>8</v>
@@ -10116,7 +10116,7 @@
     </row>
     <row r="83" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A83" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B83" s="1" t="s">
         <v>9</v>
@@ -10139,7 +10139,7 @@
     </row>
     <row r="84" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A84" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B84" s="1" t="s">
         <v>0</v>
@@ -10162,7 +10162,7 @@
     </row>
     <row r="85" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A85" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B85" s="1" t="s">
         <v>1</v>
@@ -10185,7 +10185,7 @@
     </row>
     <row r="86" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A86" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B86" s="1" t="s">
         <v>2</v>
@@ -10208,7 +10208,7 @@
     </row>
     <row r="87" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A87" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B87" s="1" t="s">
         <v>3</v>
@@ -10231,7 +10231,7 @@
     </row>
     <row r="88" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A88" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B88" s="1" t="s">
         <v>4</v>
@@ -10254,7 +10254,7 @@
     </row>
     <row r="89" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A89" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B89" s="1" t="s">
         <v>5</v>
@@ -10277,7 +10277,7 @@
     </row>
     <row r="90" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A90" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B90" s="1" t="s">
         <v>6</v>
@@ -10300,7 +10300,7 @@
     </row>
     <row r="91" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A91" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B91" s="1" t="s">
         <v>7</v>
@@ -10323,7 +10323,7 @@
     </row>
     <row r="92" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A92" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B92" s="1" t="s">
         <v>8</v>
@@ -10346,7 +10346,7 @@
     </row>
     <row r="93" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A93" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B93" s="1" t="s">
         <v>9</v>
@@ -10369,7 +10369,7 @@
     </row>
     <row r="94" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A94" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B94" s="1" t="s">
         <v>0</v>
@@ -10392,7 +10392,7 @@
     </row>
     <row r="95" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A95" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B95" s="1" t="s">
         <v>1</v>
@@ -10415,7 +10415,7 @@
     </row>
     <row r="96" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A96" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B96" s="1" t="s">
         <v>2</v>
@@ -10438,7 +10438,7 @@
     </row>
     <row r="97" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A97" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B97" s="1" t="s">
         <v>3</v>
@@ -10461,7 +10461,7 @@
     </row>
     <row r="98" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A98" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B98" s="1" t="s">
         <v>4</v>
@@ -10484,7 +10484,7 @@
     </row>
     <row r="99" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A99" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B99" s="1" t="s">
         <v>5</v>
@@ -10507,7 +10507,7 @@
     </row>
     <row r="100" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A100" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B100" s="1" t="s">
         <v>6</v>
@@ -10530,7 +10530,7 @@
     </row>
     <row r="101" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A101" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B101" s="1" t="s">
         <v>7</v>
@@ -10553,7 +10553,7 @@
     </row>
     <row r="102" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A102" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B102" s="1" t="s">
         <v>8</v>
@@ -10576,7 +10576,7 @@
     </row>
     <row r="103" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A103" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B103" s="1" t="s">
         <v>9</v>
@@ -10599,7 +10599,7 @@
     </row>
     <row r="104" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A104" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B104" s="1" t="s">
         <v>0</v>
@@ -10622,7 +10622,7 @@
     </row>
     <row r="105" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A105" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B105" s="1" t="s">
         <v>1</v>
@@ -10645,7 +10645,7 @@
     </row>
     <row r="106" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A106" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B106" s="1" t="s">
         <v>2</v>
@@ -10668,7 +10668,7 @@
     </row>
     <row r="107" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A107" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B107" s="1" t="s">
         <v>3</v>
@@ -10691,7 +10691,7 @@
     </row>
     <row r="108" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A108" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B108" s="1" t="s">
         <v>4</v>
@@ -10714,7 +10714,7 @@
     </row>
     <row r="109" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A109" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B109" s="1" t="s">
         <v>5</v>
@@ -10737,7 +10737,7 @@
     </row>
     <row r="110" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A110" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B110" s="1" t="s">
         <v>6</v>
@@ -10760,7 +10760,7 @@
     </row>
     <row r="111" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A111" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B111" s="1" t="s">
         <v>7</v>
@@ -10783,7 +10783,7 @@
     </row>
     <row r="112" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A112" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B112" s="1" t="s">
         <v>8</v>
@@ -10806,7 +10806,7 @@
     </row>
     <row r="113" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A113" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B113" s="1" t="s">
         <v>9</v>
@@ -10829,7 +10829,7 @@
     </row>
     <row r="114" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A114" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B114" s="1" t="s">
         <v>0</v>
@@ -10852,7 +10852,7 @@
     </row>
     <row r="115" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A115" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B115" s="1" t="s">
         <v>1</v>
@@ -10875,7 +10875,7 @@
     </row>
     <row r="116" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A116" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B116" s="1" t="s">
         <v>2</v>
@@ -10898,7 +10898,7 @@
     </row>
     <row r="117" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A117" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B117" s="1" t="s">
         <v>3</v>
@@ -10921,7 +10921,7 @@
     </row>
     <row r="118" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A118" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B118" s="1" t="s">
         <v>4</v>
@@ -10944,7 +10944,7 @@
     </row>
     <row r="119" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A119" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B119" s="1" t="s">
         <v>5</v>
@@ -10967,7 +10967,7 @@
     </row>
     <row r="120" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A120" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B120" s="1" t="s">
         <v>6</v>
@@ -10990,7 +10990,7 @@
     </row>
     <row r="121" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A121" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B121" s="1" t="s">
         <v>7</v>
@@ -11013,7 +11013,7 @@
     </row>
     <row r="122" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A122" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B122" s="1" t="s">
         <v>8</v>
@@ -11036,7 +11036,7 @@
     </row>
     <row r="123" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A123" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B123" s="1" t="s">
         <v>9</v>
@@ -11059,7 +11059,7 @@
     </row>
     <row r="124" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A124" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B124" s="1" t="s">
         <v>0</v>
@@ -11079,7 +11079,7 @@
     </row>
     <row r="125" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A125" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B125" s="1" t="s">
         <v>1</v>
@@ -11099,7 +11099,7 @@
     </row>
     <row r="126" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A126" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B126" s="1" t="s">
         <v>2</v>
@@ -11122,7 +11122,7 @@
     </row>
     <row r="127" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A127" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B127" s="1" t="s">
         <v>3</v>
@@ -11142,7 +11142,7 @@
     </row>
     <row r="128" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A128" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B128" s="1" t="s">
         <v>4</v>
@@ -11162,7 +11162,7 @@
     </row>
     <row r="129" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A129" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B129" s="1" t="s">
         <v>5</v>
@@ -11185,7 +11185,7 @@
     </row>
     <row r="130" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A130" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B130" s="1" t="s">
         <v>6</v>
@@ -11208,7 +11208,7 @@
     </row>
     <row r="131" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A131" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B131" s="1" t="s">
         <v>7</v>
@@ -11231,7 +11231,7 @@
     </row>
     <row r="132" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A132" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B132" s="1" t="s">
         <v>8</v>
@@ -11254,7 +11254,7 @@
     </row>
     <row r="133" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A133" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B133" s="1" t="s">
         <v>9</v>
@@ -11274,7 +11274,7 @@
     </row>
     <row r="134" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A134" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B134" s="1" t="s">
         <v>0</v>
@@ -11288,7 +11288,7 @@
     </row>
     <row r="135" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A135" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B135" s="1" t="s">
         <v>1</v>
@@ -11302,7 +11302,7 @@
     </row>
     <row r="136" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A136" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B136" s="1" t="s">
         <v>2</v>
@@ -11325,7 +11325,7 @@
     </row>
     <row r="137" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A137" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B137" s="1" t="s">
         <v>3</v>
@@ -11339,7 +11339,7 @@
     </row>
     <row r="138" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A138" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B138" s="1" t="s">
         <v>4</v>
@@ -11353,7 +11353,7 @@
     </row>
     <row r="139" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A139" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B139" s="1" t="s">
         <v>5</v>
@@ -11373,7 +11373,7 @@
     </row>
     <row r="140" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A140" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B140" s="1" t="s">
         <v>6</v>
@@ -11396,7 +11396,7 @@
     </row>
     <row r="141" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A141" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B141" s="1" t="s">
         <v>7</v>
@@ -11419,7 +11419,7 @@
     </row>
     <row r="142" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A142" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B142" s="1" t="s">
         <v>8</v>
@@ -11439,7 +11439,7 @@
     </row>
     <row r="143" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A143" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B143" s="1" t="s">
         <v>9</v>
@@ -11456,7 +11456,7 @@
     </row>
     <row r="144" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A144" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B144" s="1" t="s">
         <v>0</v>
@@ -11470,7 +11470,7 @@
     </row>
     <row r="145" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A145" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B145" s="1" t="s">
         <v>1</v>
@@ -11484,7 +11484,7 @@
     </row>
     <row r="146" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A146" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B146" s="1" t="s">
         <v>2</v>
@@ -11504,7 +11504,7 @@
     </row>
     <row r="147" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A147" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B147" s="1" t="s">
         <v>3</v>
@@ -11518,7 +11518,7 @@
     </row>
     <row r="148" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A148" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B148" s="1" t="s">
         <v>4</v>
@@ -11532,7 +11532,7 @@
     </row>
     <row r="149" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A149" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B149" s="1" t="s">
         <v>5</v>
@@ -11549,7 +11549,7 @@
     </row>
     <row r="150" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A150" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B150" s="1" t="s">
         <v>6</v>
@@ -11569,7 +11569,7 @@
     </row>
     <row r="151" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A151" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B151" s="1" t="s">
         <v>7</v>
@@ -11589,7 +11589,7 @@
     </row>
     <row r="152" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A152" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B152" s="1" t="s">
         <v>8</v>
@@ -11603,7 +11603,7 @@
     </row>
     <row r="153" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A153" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B153" s="1" t="s">
         <v>9</v>
@@ -11617,7 +11617,7 @@
     </row>
     <row r="154" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A154" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B154" s="1" t="s">
         <v>0</v>
@@ -11631,7 +11631,7 @@
     </row>
     <row r="155" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A155" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B155" s="1" t="s">
         <v>1</v>
@@ -11645,7 +11645,7 @@
     </row>
     <row r="156" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A156" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B156" s="1" t="s">
         <v>2</v>
@@ -11659,7 +11659,7 @@
     </row>
     <row r="157" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A157" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B157" s="1" t="s">
         <v>3</v>
@@ -11673,7 +11673,7 @@
     </row>
     <row r="158" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A158" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B158" s="1" t="s">
         <v>4</v>
@@ -11687,7 +11687,7 @@
     </row>
     <row r="159" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A159" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B159" s="1" t="s">
         <v>5</v>
@@ -11701,7 +11701,7 @@
     </row>
     <row r="160" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A160" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B160" s="1" t="s">
         <v>6</v>
@@ -11715,7 +11715,7 @@
     </row>
     <row r="161" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A161" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B161" s="1" t="s">
         <v>7</v>
@@ -11729,7 +11729,7 @@
     </row>
     <row r="162" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A162" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B162" s="1" t="s">
         <v>8</v>
@@ -11743,7 +11743,7 @@
     </row>
     <row r="163" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A163" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B163" s="1" t="s">
         <v>9</v>
@@ -11757,7 +11757,7 @@
     </row>
     <row r="164" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A164" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B164" s="1" t="s">
         <v>0</v>
@@ -11771,7 +11771,7 @@
     </row>
     <row r="165" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A165" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B165" s="1" t="s">
         <v>1</v>
@@ -11785,7 +11785,7 @@
     </row>
     <row r="166" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A166" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B166" s="1" t="s">
         <v>2</v>
@@ -11799,7 +11799,7 @@
     </row>
     <row r="167" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A167" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B167" s="1" t="s">
         <v>3</v>
@@ -11813,7 +11813,7 @@
     </row>
     <row r="168" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A168" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B168" s="1" t="s">
         <v>4</v>
@@ -11827,7 +11827,7 @@
     </row>
     <row r="169" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A169" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B169" s="1" t="s">
         <v>5</v>
@@ -11841,7 +11841,7 @@
     </row>
     <row r="170" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A170" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B170" s="1" t="s">
         <v>6</v>
@@ -11855,7 +11855,7 @@
     </row>
     <row r="171" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A171" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B171" s="1" t="s">
         <v>7</v>
@@ -11869,7 +11869,7 @@
     </row>
     <row r="172" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A172" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B172" s="1" t="s">
         <v>8</v>
@@ -11883,7 +11883,7 @@
     </row>
     <row r="173" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A173" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B173" s="1" t="s">
         <v>9</v>
@@ -11897,7 +11897,7 @@
     </row>
     <row r="174" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A174" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B174" s="1" t="s">
         <v>0</v>
@@ -11911,7 +11911,7 @@
     </row>
     <row r="175" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A175" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B175" s="1" t="s">
         <v>1</v>
@@ -11925,7 +11925,7 @@
     </row>
     <row r="176" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A176" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B176" s="1" t="s">
         <v>2</v>
@@ -11939,7 +11939,7 @@
     </row>
     <row r="177" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A177" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B177" s="1" t="s">
         <v>3</v>
@@ -11953,7 +11953,7 @@
     </row>
     <row r="178" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A178" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B178" s="1" t="s">
         <v>4</v>
@@ -11967,7 +11967,7 @@
     </row>
     <row r="179" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A179" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B179" s="1" t="s">
         <v>5</v>
@@ -11981,7 +11981,7 @@
     </row>
     <row r="180" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A180" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B180" s="1" t="s">
         <v>6</v>
@@ -11995,7 +11995,7 @@
     </row>
     <row r="181" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A181" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B181" s="1" t="s">
         <v>7</v>
@@ -12009,7 +12009,7 @@
     </row>
     <row r="182" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A182" s="1" t="s">
-        <v>26</v>
+        <v>22</v>
       </c>
       <c r="B182" s="1" t="s">
         <v>8</v>
@@ -12020,7 +12020,7 @@
     </row>
     <row r="183" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A183" s="1" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B183" s="1" t="s">
         <v>9</v>
@@ -12031,7 +12031,7 @@
     </row>
     <row r="184" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A184" s="1" t="s">
-        <v>28</v>
+        <v>24</v>
       </c>
       <c r="B184" s="1" t="s">
         <v>0</v>
@@ -12042,7 +12042,7 @@
     </row>
     <row r="185" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A185" s="1" t="s">
-        <v>29</v>
+        <v>25</v>
       </c>
       <c r="B185" s="1" t="s">
         <v>1</v>
@@ -12056,7 +12056,7 @@
     </row>
     <row r="186" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A186" s="1" t="s">
-        <v>30</v>
+        <v>26</v>
       </c>
       <c r="B186" s="1" t="s">
         <v>2</v>
@@ -12070,7 +12070,7 @@
     </row>
     <row r="187" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A187" s="1" t="s">
-        <v>31</v>
+        <v>27</v>
       </c>
       <c r="B187" s="1" t="s">
         <v>3</v>
@@ -12081,7 +12081,7 @@
     </row>
     <row r="188" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A188" s="1" t="s">
-        <v>32</v>
+        <v>28</v>
       </c>
       <c r="B188" s="1" t="s">
         <v>4</v>
@@ -12092,7 +12092,7 @@
     </row>
     <row r="189" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A189" s="1" t="s">
-        <v>33</v>
+        <v>29</v>
       </c>
       <c r="B189" s="1" t="s">
         <v>5</v>
@@ -12103,7 +12103,7 @@
     </row>
     <row r="190" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A190" s="1" t="s">
-        <v>34</v>
+        <v>30</v>
       </c>
       <c r="B190" s="1" t="s">
         <v>6</v>
@@ -12114,7 +12114,7 @@
     </row>
     <row r="191" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A191" s="1" t="s">
-        <v>35</v>
+        <v>31</v>
       </c>
       <c r="B191" s="1" t="s">
         <v>7</v>

</xml_diff>